<commit_message>
create-chart ms-- the parsers
The chart parsers are used to take the data the user provided and create their chart
</commit_message>
<xml_diff>
--- a/microservices/download templates/src/templatesStorage/dependencyWheelTemplate.xlsx
+++ b/microservices/download templates/src/templatesStorage/dependencyWheelTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORA\Documents\GitHub\SaaS23-60\microservices\download templates\src\templatesStorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F497F7B-0239-4296-AF39-1A3D7265368E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CD6D060-47B6-4B3E-9D5F-6B2001E2204D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46EB44D5-4E4C-4FBF-9B9B-9B8682C03FE5}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Chart's Title</t>
   </si>
   <si>
-    <t>examleTitle</t>
-  </si>
-  <si>
     <t>Chart Data</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>dependencyWheel</t>
+  </si>
+  <si>
+    <t>YourTitle</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:BY462"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,7 +499,7 @@
   <sheetData>
     <row r="1" spans="1:77" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:77" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
@@ -507,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -515,26 +515,26 @@
     </row>
     <row r="3" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:77" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:77" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="5" spans="1:77" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:77" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>